<commit_message>
commit right before the arena/editmode/game/lobby rework
</commit_message>
<xml_diff>
--- a/BattleGrounds TODO.xlsx
+++ b/BattleGrounds TODO.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Priority</t>
   </si>
@@ -27,28 +27,10 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Refine Arena Creation
-- Better feedback</t>
-  </si>
-  <si>
-    <t>Implement ArrayList of creatureSpawns</t>
-  </si>
-  <si>
-    <t>Implement ArrayList of playerSpawns</t>
-  </si>
-  <si>
     <t>Overhaul commandHandler</t>
   </si>
   <si>
     <t>BATTLEGROUNDS TODO LIST</t>
-  </si>
-  <si>
-    <t>new Thread for new GameHandlers
-- Allows us to have delays in rounds/games
-- Listener for each game outside game thread (register on game-start, unregister on game-end)
-- Save original Location before /bg join [arena] command for use later
-- Save items and gamemode on game join, then wipe inventory
-- Restore items, gamemode and location on game leave</t>
   </si>
 </sst>
 </file>
@@ -513,7 +495,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="8" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B1" s="8"/>
     </row>
@@ -525,35 +507,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
-      <c r="B3" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="B3" s="3"/>
     </row>
     <row r="4" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
-      <c r="B4" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B4" s="3"/>
     </row>
     <row r="5" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
-      <c r="B5" s="3" t="s">
-        <v>4</v>
-      </c>
+      <c r="B5" s="3"/>
     </row>
     <row r="6" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
-      <c r="B7" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="B7" s="3"/>
     </row>
     <row r="8" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>

</xml_diff>